<commit_message>
Added date parsing to ExcelExtractor(85397)
</commit_message>
<xml_diff>
--- a/src/test/resources/test-extract1.xlsx
+++ b/src/test/resources/test-extract1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="12800" windowHeight="8040"/>
+    <workbookView activeTab="0" windowWidth="13660" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -41,6 +41,16 @@
       <name val="Sans"/>
       <vertAlign val="baseline"/>
       <sz val="10"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <u val="none"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <vertAlign val="baseline"/>
+      <sz val="11"/>
       <strike val="0"/>
     </font>
     <font>
@@ -54,15 +64,21 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="0" diagonalDown="0">
       <left style="none">
         <color rgb="FFC7C7C7"/>
@@ -75,6 +91,20 @@
       </top>
       <bottom style="none">
         <color rgb="FFC7C7C7"/>
+      </bottom>
+    </border>
+    <border diagonalUp="0" diagonalDown="0">
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
     </border>
   </borders>
@@ -83,11 +113,14 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="1" numFmtId="14" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
@@ -99,15 +132,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="4" style="0" width="9.142308"/>
+    <col min="1" max="1" style="0" width="10.71364" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" style="0" width="9.142308"/>
     <col min="5" max="16384" style="0"/>
   </cols>
   <sheetData>
@@ -141,10 +175,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" customHeight="1" ht="32.25">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>a4</t>
-        </is>
+      <c r="A4" s="1">
+        <v>43252</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -187,7 +219,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -219,7 +251,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>